<commit_message>
updates to databases and immpex scripts
</commit_message>
<xml_diff>
--- a/files/Cemdata18/source/discretization/CSH20-alkalis2.xlsx
+++ b/files/Cemdata18/source/discretization/CSH20-alkalis2.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="191">
   <si>
     <t xml:space="preserve">symbol</t>
   </si>
@@ -244,25 +244,7 @@
     <t xml:space="preserve">CSH077+N0318</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">CSH080+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">N0000</t>
-    </r>
+    <t xml:space="preserve">CSH080+N0000</t>
   </si>
   <si>
     <t xml:space="preserve">CSH081+N0064</t>
@@ -277,25 +259,7 @@
     <t xml:space="preserve">CSH081+N0324</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">CSH089+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">N0000</t>
-    </r>
+    <t xml:space="preserve">CSH089+N0000</t>
   </si>
   <si>
     <t xml:space="preserve">CSH090+N0048</t>
@@ -310,25 +274,7 @@
     <t xml:space="preserve">CSH090+N0302</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">CSH098+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">N0000</t>
-    </r>
+    <t xml:space="preserve">CSH098+N0000</t>
   </si>
   <si>
     <t xml:space="preserve">CSH099+N0041</t>
@@ -343,25 +289,7 @@
     <t xml:space="preserve">CSH099+N0274</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">CSH106+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">N0000</t>
-    </r>
+    <t xml:space="preserve">CSH106+N0000</t>
   </si>
   <si>
     <t xml:space="preserve">CSH108+N0036</t>
@@ -376,25 +304,7 @@
     <t xml:space="preserve">CSH109+N0248</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">CSH115+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">N0000</t>
-    </r>
+    <t xml:space="preserve">CSH115+N0000</t>
   </si>
   <si>
     <t xml:space="preserve">CSH118+N0034</t>
@@ -409,25 +319,7 @@
     <t xml:space="preserve">CSH118+N0222</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">CSH123+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">N0000</t>
-    </r>
+    <t xml:space="preserve">CSH123+N0000</t>
   </si>
   <si>
     <t xml:space="preserve">CSH127+N0033</t>
@@ -442,25 +334,7 @@
     <t xml:space="preserve">CSH127+N0196</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">CSH132+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">N0000</t>
-    </r>
+    <t xml:space="preserve">CSH132+N0000</t>
   </si>
   <si>
     <t xml:space="preserve">CSH136+N0029</t>
@@ -475,25 +349,7 @@
     <t xml:space="preserve">CSH137+N0169</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">CSH140+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">N0000</t>
-    </r>
+    <t xml:space="preserve">CSH140+N0000</t>
   </si>
   <si>
     <t xml:space="preserve">CSH145+N0025</t>
@@ -704,6 +560,30 @@
   </si>
   <si>
     <t xml:space="preserve">CSH163+K0072</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ca    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">H     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Na    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">O     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zz    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">a   aq_gen          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">s   CASH+           </t>
   </si>
   <si>
     <t xml:space="preserve">R3 ( CSH071+A00102 + 4.2352H+ + 0.0003e- = 2.9248SiO2@ + 5.2351H2O@ + 2.0729Ca+2 + 0.0297Al+3 )</t>
@@ -728,7 +608,7 @@
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
     <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -750,12 +630,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -845,9 +719,9 @@
   <dimension ref="A1:AQ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="K101" activeCellId="0" sqref="K101:L155"/>
+      <selection pane="bottomLeft" activeCell="T160" activeCellId="0" sqref="T160:U160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15048,6 +14922,246 @@
       <c r="AC155" s="0" t="n">
         <f aca="false">J155-2*AA155-ROUND(E155,4)</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S157" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="T157" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="V157" s="0" t="n">
+        <f aca="false">W157*S157</f>
+        <v>0.8</v>
+      </c>
+      <c r="W157" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X157" s="0" t="n">
+        <f aca="false">W157*T157</f>
+        <v>0.1</v>
+      </c>
+      <c r="AA157" s="0" t="n">
+        <v>1.165</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B158" s="1" t="n">
+        <f aca="false">F158/G158</f>
+        <v>0.80971358340151</v>
+      </c>
+      <c r="C158" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("Ca", ROUND(F158, 4), "Si",ROUND(G158, 4), "Na",ROUND(E158, 4), "O",ROUND(H158, 4), "H",J158)</f>
+        <v>Ca2.1675Si2.6769Na0.3803O11.0684H6.7139</v>
+      </c>
+      <c r="E158" s="3" t="n">
+        <v>0.380286</v>
+      </c>
+      <c r="F158" s="3" t="n">
+        <v>2.167498</v>
+      </c>
+      <c r="G158" s="3" t="n">
+        <v>2.67687</v>
+      </c>
+      <c r="H158" s="3" t="n">
+        <v>11.06839</v>
+      </c>
+      <c r="I158" s="3" t="n">
+        <v>6.714021</v>
+      </c>
+      <c r="J158" s="0" t="n">
+        <f aca="false">I158-AB158</f>
+        <v>6.7139</v>
+      </c>
+      <c r="K158" s="3" t="n">
+        <v>0.354648</v>
+      </c>
+      <c r="L158" s="3" t="n">
+        <v>13.48103</v>
+      </c>
+      <c r="M158" s="3" t="n">
+        <v>-4697.66</v>
+      </c>
+      <c r="N158" s="3" t="n">
+        <v>-4697.66</v>
+      </c>
+      <c r="O158" s="3" t="n">
+        <v>-5102.567</v>
+      </c>
+      <c r="P158" s="3" t="n">
+        <v>-7.385915</v>
+      </c>
+      <c r="Q158" s="3" t="n">
+        <v>338.9487</v>
+      </c>
+      <c r="R158" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("CSH", S158, "+N",T158)</f>
+        <v>CSH0.81+N0.142</v>
+      </c>
+      <c r="S158" s="1" t="n">
+        <f aca="false">ROUND(B158,2)</f>
+        <v>0.81</v>
+      </c>
+      <c r="T158" s="4" t="n">
+        <f aca="false">ROUND(E158/G158,3)</f>
+        <v>0.142</v>
+      </c>
+      <c r="U158" s="1"/>
+      <c r="V158" s="0" t="n">
+        <f aca="false">W158*S158</f>
+        <v>0.81</v>
+      </c>
+      <c r="W158" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X158" s="0" t="n">
+        <f aca="false">W158*T158</f>
+        <v>0.142</v>
+      </c>
+      <c r="Z158" s="0" t="n">
+        <f aca="false">ROUND(H158,4)-2*ROUND(G158,4)-ROUND(F158,4)-ROUND(E158,4)</f>
+        <v>3.1668</v>
+      </c>
+      <c r="AA158" s="0" t="n">
+        <f aca="false">ROUND(Z158,4)</f>
+        <v>3.1668</v>
+      </c>
+      <c r="AB158" s="0" t="n">
+        <f aca="false">I158-2*AA158-ROUND(E158,4)</f>
+        <v>0.000121000000000093</v>
+      </c>
+      <c r="AC158" s="0" t="n">
+        <f aca="false">J158-2*AA158-ROUND(E158,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T159" s="0" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="U159" s="0" t="n">
+        <f aca="false">LOG10(T159)</f>
+        <v>-4</v>
+      </c>
+      <c r="AA159" s="0" t="n">
+        <f aca="false">AA158/2</f>
+        <v>1.5834</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T160" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="U160" s="0" t="n">
+        <f aca="false">LOG10(T160)</f>
+        <v>-0.301029995663981</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T161" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="U161" s="0" t="n">
+        <f aca="false">LOG10(T161)</f>
+        <v>-0.522878745280338</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M165" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="N165" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="O165" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="P165" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q165" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="R165" s="0" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M166" s="0" t="n">
+        <v>0.80999855</v>
+      </c>
+      <c r="N166" s="0" t="n">
+        <v>2.5082192</v>
+      </c>
+      <c r="O166" s="0" t="n">
+        <v>0.14160407</v>
+      </c>
+      <c r="P166" s="0" t="n">
+        <v>4.1348266</v>
+      </c>
+      <c r="Q166" s="0" t="n">
+        <v>0.9999582</v>
+      </c>
+      <c r="R166" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M167" s="2" t="n">
+        <v>1.4509909E-006</v>
+      </c>
+      <c r="N167" s="0" t="n">
+        <v>1.6337808</v>
+      </c>
+      <c r="O167" s="0" t="n">
+        <v>0.00039593461</v>
+      </c>
+      <c r="P167" s="0" t="n">
+        <v>0.8171734</v>
+      </c>
+      <c r="Q167" s="2" t="n">
+        <v>4.1802261E-005</v>
+      </c>
+      <c r="R167" s="2" t="n">
+        <v>-5.3508623E-016</v>
+      </c>
+      <c r="S167" s="0" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M168" s="0" t="n">
+        <v>0.80999855</v>
+      </c>
+      <c r="N168" s="0" t="n">
+        <v>2.5082192</v>
+      </c>
+      <c r="O168" s="0" t="n">
+        <v>0.14160407</v>
+      </c>
+      <c r="P168" s="0" t="n">
+        <v>4.1348266</v>
+      </c>
+      <c r="Q168" s="0" t="n">
+        <v>0.9999582</v>
+      </c>
+      <c r="R168" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S168" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="T168" s="0" t="n">
+        <f aca="false">P168-M168-2*Q168-O168</f>
+        <v>1.18330758</v>
+      </c>
+      <c r="U168" s="0" t="n">
+        <f aca="false">(N168-O168)/2</f>
+        <v>1.183307565</v>
       </c>
     </row>
     <row r="1048504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -15142,7 +15256,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="1" sqref="K101:L155 E7"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="1" sqref="T160:U160 E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15153,13 +15267,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="D1" s="0" t="n">
         <v>26.727</v>
@@ -15182,7 +15296,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>8</v>
@@ -15263,14 +15377,14 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="E6" s="0" t="n">
         <f aca="false">4.2352</f>
         <v>4.2352</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="K6" s="0" t="n">
         <f aca="false">I5+K5</f>
@@ -15296,7 +15410,7 @@
   <dimension ref="A1:A36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="K101:L155 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="T160:U160 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15539,7 +15653,7 @@
   <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B55" activeCellId="1" sqref="K101:L155 B55"/>
+      <selection pane="topLeft" activeCell="B55" activeCellId="1" sqref="T160:U160 B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>